<commit_message>
Bổ sung tính ẩn hiện hướng dẫn (F1). Thêm âm thanh cho phần chọn trong Load game. Cập nhật báo cáo.
</commit_message>
<xml_diff>
--- a/0812515_0812527/Reference/ChecklistReference.xlsx
+++ b/0812515_0812527/Reference/ChecklistReference.xlsx
@@ -39,18 +39,12 @@
     <t>Các tập tin hình ảnh (jpg)</t>
   </si>
   <si>
-    <t>EKOS MP3Minimizer</t>
-  </si>
-  <si>
     <t>Resource cung cấp trong môn học C4W</t>
   </si>
   <si>
     <t>Thu âm</t>
   </si>
   <si>
-    <t>Mp3 Audio Editor</t>
-  </si>
-  <si>
     <t>Các demo xử lý</t>
   </si>
   <si>
@@ -67,6 +61,12 @@
   </si>
   <si>
     <t>Nơi tham khảo</t>
+  </si>
+  <si>
+    <t>Phần mềm EKOS MP3Minimizer</t>
+  </si>
+  <si>
+    <t>Phần mềm Mp3 Audio Editor</t>
   </si>
 </sst>
 </file>
@@ -209,38 +209,38 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -550,81 +550,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="3" t="s">
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="5" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="9"/>
+      <c r="B8" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="4" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="6" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="7" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>